<commit_message>
- CHG: Moved any type definitions/lookups/validations to a separate TYPES sheet.
</commit_message>
<xml_diff>
--- a/environmental-data/environmental-data.xlsx
+++ b/environmental-data/environmental-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\environmental-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B7A888-94B2-4471-A591-039FCB622EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56143088-40D1-4411-BE6E-B147B4D1E20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,9 +19,10 @@
     <sheet name="ATTRIBUTES" sheetId="11" r:id="rId4"/>
     <sheet name="COLLABORATORS" sheetId="9" r:id="rId5"/>
     <sheet name="LOCATION" sheetId="12" r:id="rId6"/>
-    <sheet name="LOCATION_EXAMPLE" sheetId="13" r:id="rId7"/>
-    <sheet name="ENVIRONMENTAL VARIABLES_EXAMPLE" sheetId="5" r:id="rId8"/>
-    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId9"/>
+    <sheet name="TYPES" sheetId="14" r:id="rId7"/>
+    <sheet name="LOCATION_EXAMPLE" sheetId="13" r:id="rId8"/>
+    <sheet name="ENVIRONMENTAL VARIABLES_EXAMPLE" sheetId="5" r:id="rId9"/>
+    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +217,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>ValidTypes</t>
   </si>
   <si>
     <t>Location/Climate</t>
@@ -603,9 +601,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -617,17 +613,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -652,7 +643,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -686,9 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -700,6 +688,27 @@
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -805,20 +814,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -912,13 +907,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -959,12 +947,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{708F31BA-D14C-48D2-B473-BC6BB16FAB35}" name="Table710" displayName="Table710" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{708F31BA-D14C-48D2-B473-BC6BB16FAB35}" name="Table710" displayName="Table710" ref="A1:C18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:C18" xr:uid="{708F31BA-D14C-48D2-B473-BC6BB16FAB35}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C6B5B326-9F6D-405F-B82D-C4B296BD80CE}" name="LABEL" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C4C3E759-E46C-443D-8710-89F747B5FEBF}" name="DEFINITION" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{C79B25D2-E319-4610-A399-99865CC83370}" name="VALUE" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{C6B5B326-9F6D-405F-B82D-C4B296BD80CE}" name="LABEL" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{C4C3E759-E46C-443D-8710-89F747B5FEBF}" name="DEFINITION" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{C79B25D2-E319-4610-A399-99865CC83370}" name="VALUE" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -991,7 +979,7 @@
   <autoFilter ref="A1:B2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CCD80E05-5388-423E-BBDC-2354AB7B8FC3}" name="Location/Climate"/>
-    <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Date" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Date" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,18 +998,18 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{1DA7637C-C056-4913-BCA6-9B3815700BDE}" name="Contributor role" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{AA69BB00-B8A2-4F9B-A718-91811DE74929}" name="Contributor ID" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{1DA7637C-C056-4913-BCA6-9B3815700BDE}" name="Contributor role" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{AA69BB00-B8A2-4F9B-A718-91811DE74929}" name="Contributor ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1043,6 +1031,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B500507A-024E-435D-A17B-E346A72090D6}" name="Table7" displayName="Table7" ref="A1:A5" totalsRowShown="0">
+  <autoFilter ref="A1:A5" xr:uid="{B500507A-024E-435D-A17B-E346A72090D6}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{CE6C49C4-8999-4BB8-A742-415067083C4A}" name="Possible data types"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4D8FF69F-94D5-4732-82EA-A3B39E460300}" name="Table95" displayName="Table95" ref="A1:F3" totalsRowShown="0">
   <autoFilter ref="A1:F3" xr:uid="{4E2C0938-9EE0-4C04-8B7D-6D0F8EF95120}"/>
   <tableColumns count="6">
@@ -1057,7 +1055,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G7" totalsRowShown="0">
   <autoFilter ref="A1:G7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
@@ -1344,225 +1342,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="5" max="5" width="13.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="13.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="C13" s="37"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="43"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="B14" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="C14" s="37"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="43"/>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="B15" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="C15" s="37"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="43"/>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="B16" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="C16" s="37"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="43"/>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="B17" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="C17" s="37"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="43"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="B18" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="11" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="24" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1574,12 +1567,582 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="29">
+        <v>71.257798170000001</v>
+      </c>
+      <c r="D2" s="29">
+        <v>12.857889910000001</v>
+      </c>
+      <c r="E2" s="29">
+        <v>28.588073390000002</v>
+      </c>
+      <c r="F2" s="29">
+        <v>4.686238532</v>
+      </c>
+      <c r="G2" s="30">
+        <v>21.490825690000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="33">
+        <v>71.166972479999998</v>
+      </c>
+      <c r="D3" s="33">
+        <v>15.392110089999999</v>
+      </c>
+      <c r="E3" s="33">
+        <v>13.367889910000001</v>
+      </c>
+      <c r="F3" s="33">
+        <v>6.473394495</v>
+      </c>
+      <c r="G3" s="34">
+        <v>22.334862390000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="29">
+        <v>81.969724769999999</v>
+      </c>
+      <c r="D4" s="29">
+        <v>25.25174312</v>
+      </c>
+      <c r="E4" s="29">
+        <v>25.807339450000001</v>
+      </c>
+      <c r="F4" s="29">
+        <v>5.288990826</v>
+      </c>
+      <c r="G4" s="30">
+        <v>22.637614679999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="33">
+        <v>65.707339450000006</v>
+      </c>
+      <c r="D5" s="33">
+        <v>25.722568809999999</v>
+      </c>
+      <c r="E5" s="33">
+        <v>21.129357800000001</v>
+      </c>
+      <c r="F5" s="33">
+        <v>5.4889908260000002</v>
+      </c>
+      <c r="G5" s="34">
+        <v>25.15045872</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="29">
+        <v>74.703669719999994</v>
+      </c>
+      <c r="D6" s="29">
+        <v>30.143669719999998</v>
+      </c>
+      <c r="E6" s="29">
+        <v>30.366972480000001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>5.923853211</v>
+      </c>
+      <c r="G6" s="30">
+        <v>24.01743119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="33">
+        <v>73.083486239999999</v>
+      </c>
+      <c r="D7" s="33">
+        <v>27.937798170000001</v>
+      </c>
+      <c r="E7" s="33">
+        <v>30</v>
+      </c>
+      <c r="F7" s="33">
+        <v>5.6522935780000001</v>
+      </c>
+      <c r="G7" s="34">
+        <v>25.149541280000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="29">
+        <v>72.968807339999998</v>
+      </c>
+      <c r="D8" s="29">
+        <v>20.827431189999999</v>
+      </c>
+      <c r="E8" s="29">
+        <v>12.22844037</v>
+      </c>
+      <c r="F8" s="29">
+        <v>5.7211009170000002</v>
+      </c>
+      <c r="G8" s="30">
+        <v>23.60642202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="33">
+        <v>76.782568810000001</v>
+      </c>
+      <c r="D9" s="33">
+        <v>14.12577982</v>
+      </c>
+      <c r="E9" s="33">
+        <v>30.302752290000001</v>
+      </c>
+      <c r="F9" s="33">
+        <v>6.2321100920000001</v>
+      </c>
+      <c r="G9" s="34">
+        <v>22.39357798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="29">
+        <v>71.926605499999994</v>
+      </c>
+      <c r="D10" s="29">
+        <v>18.799449540000001</v>
+      </c>
+      <c r="E10" s="29">
+        <v>31.0293578</v>
+      </c>
+      <c r="F10" s="29">
+        <v>5.1724770639999997</v>
+      </c>
+      <c r="G10" s="30">
+        <v>24.786238529999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="33">
+        <v>68.669724770000002</v>
+      </c>
+      <c r="D11" s="33">
+        <v>30.9287156</v>
+      </c>
+      <c r="E11" s="33">
+        <v>31.1</v>
+      </c>
+      <c r="F11" s="33">
+        <v>5.2853211010000001</v>
+      </c>
+      <c r="G11" s="34">
+        <v>26.860550459999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="29">
+        <v>81.202752290000006</v>
+      </c>
+      <c r="D12" s="29">
+        <v>17.95376147</v>
+      </c>
+      <c r="E12" s="29">
+        <v>26.63853211</v>
+      </c>
+      <c r="F12" s="29">
+        <v>5.2532110090000002</v>
+      </c>
+      <c r="G12" s="30">
+        <v>21.932110089999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="33">
+        <v>70.068807340000006</v>
+      </c>
+      <c r="D13" s="33">
+        <v>19.010183489999999</v>
+      </c>
+      <c r="E13" s="33">
+        <v>31</v>
+      </c>
+      <c r="F13" s="33">
+        <v>5.4633027519999997</v>
+      </c>
+      <c r="G13" s="34">
+        <v>25.90825688</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="29">
+        <v>76.370642200000006</v>
+      </c>
+      <c r="D14" s="29">
+        <v>16.138715600000001</v>
+      </c>
+      <c r="E14" s="29">
+        <v>16.18073395</v>
+      </c>
+      <c r="F14" s="29">
+        <v>6.0357798169999999</v>
+      </c>
+      <c r="G14" s="30">
+        <v>19.023853209999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="33">
+        <v>76.220183489999997</v>
+      </c>
+      <c r="D15" s="33">
+        <v>13.73</v>
+      </c>
+      <c r="E15" s="33">
+        <v>25.331192659999999</v>
+      </c>
+      <c r="F15" s="33">
+        <v>5.7688073390000003</v>
+      </c>
+      <c r="G15" s="34">
+        <v>27.56422018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="29">
+        <v>73.533027520000005</v>
+      </c>
+      <c r="D16" s="29">
+        <v>27.46587156</v>
+      </c>
+      <c r="E16" s="29">
+        <v>31.1</v>
+      </c>
+      <c r="F16" s="29">
+        <v>5.5192660550000001</v>
+      </c>
+      <c r="G16" s="30">
+        <v>27.675229359999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="33">
+        <v>75.496330279999995</v>
+      </c>
+      <c r="D17" s="33">
+        <v>9.9022018349999996</v>
+      </c>
+      <c r="E17" s="33">
+        <v>17.3733945</v>
+      </c>
+      <c r="F17" s="33">
+        <v>5.5954128440000002</v>
+      </c>
+      <c r="G17" s="34">
+        <v>29.033027520000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="29">
+        <v>69.455045870000006</v>
+      </c>
+      <c r="D18" s="29">
+        <v>28.59174312</v>
+      </c>
+      <c r="E18" s="29">
+        <v>30.9</v>
+      </c>
+      <c r="F18" s="29">
+        <v>5.3009174310000002</v>
+      </c>
+      <c r="G18" s="30">
+        <v>20.481651379999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="33">
+        <v>82.181651380000005</v>
+      </c>
+      <c r="D19" s="33">
+        <v>17.993119270000001</v>
+      </c>
+      <c r="E19" s="33">
+        <v>14.49541284</v>
+      </c>
+      <c r="F19" s="33">
+        <v>5.5844036700000004</v>
+      </c>
+      <c r="G19" s="34">
+        <v>29.65321101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="29">
+        <v>60.251376149999999</v>
+      </c>
+      <c r="D20" s="29">
+        <v>12.321376150000001</v>
+      </c>
+      <c r="E20" s="29">
+        <v>16.60917431</v>
+      </c>
+      <c r="F20" s="29">
+        <v>6.3807339450000002</v>
+      </c>
+      <c r="G20" s="30">
+        <v>26.969724769999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="33">
+        <v>73.72752294</v>
+      </c>
+      <c r="D21" s="33">
+        <v>23.482110089999999</v>
+      </c>
+      <c r="E21" s="33">
+        <v>28.159633029999998</v>
+      </c>
+      <c r="F21" s="33">
+        <v>6.1229357799999997</v>
+      </c>
+      <c r="G21" s="34">
+        <v>23.534862390000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="29">
+        <v>72.500917430000001</v>
+      </c>
+      <c r="D22" s="29">
+        <v>11.892752290000001</v>
+      </c>
+      <c r="E22" s="29">
+        <v>29.57706422</v>
+      </c>
+      <c r="F22" s="29">
+        <v>6.1229357799999997</v>
+      </c>
+      <c r="G22" s="30">
+        <v>28.619266060000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="33">
+        <v>68.874311930000005</v>
+      </c>
+      <c r="D23" s="33">
+        <v>21.55614679</v>
+      </c>
+      <c r="E23" s="33">
+        <v>23.639449540000001</v>
+      </c>
+      <c r="F23" s="33">
+        <v>5.4935779819999997</v>
+      </c>
+      <c r="G23" s="34">
+        <v>25.710091739999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A23">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:G1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Locations on the Y axis and climates (which are described in CLIMATES tab) on the x axis. The actual climate value goes in the matrix cells. See DATA_EXAMPLE tab for more information before completion." sqref="A1" xr:uid="{FC382264-F5BB-4A0A-BB03-320EBF442EFF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Format" prompt="Dates need to be formatted in yyyy-mm-dd format, but the cell type in Excel has to be Text!" sqref="B1" xr:uid="{9F926510-BAE1-4FB0-9AC9-8B05F7299956}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I1" sqref="I1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,91 +2154,40 @@
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
     <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I5" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 D2">
-    <cfRule type="containsBlanks" dxfId="18" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="G1" xr:uid="{C6B9A6C3-B877-4AD7-A38B-42DF86B03D05}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576 D1" xr:uid="{82E3529B-0246-482A-A1C4-DA13B1AEE9F4}">
-      <formula1>$I$2:$I$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{E7F82065-00E0-406C-B1D1-FF1C0CCD1326}">
-      <formula1>$I$2:$I$5</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate Name" prompt="This should be the full name of the climate that has been recorded." sqref="A1" xr:uid="{FE8D8983-F907-4A01-AF7A-E7A8DD74798A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate Short Name" prompt="This is should be a shortened version of the climate name. This is used on some of the Germinate pages which use tables so that the climate name fits." sqref="B1" xr:uid="{25EB12EF-8D2E-4371-A2BB-C5658B595EE1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Climate Description" prompt="This should be a full description of the climate. There is no limit to the length of text that can be used here so please be descriptive." sqref="C1" xr:uid="{D755B196-EA32-42FE-9F01-EA329B60662F}"/>
@@ -1686,12 +2198,30 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{82E3529B-0246-482A-A1C4-DA13B1AEE9F4}">
+          <x14:formula1>
+            <xm:f>TYPES!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D1048576 D1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7F82065-00E0-406C-B1D1-FF1C0CCD1326}">
+          <x14:formula1>
+            <xm:f>TYPES!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
@@ -1700,53 +2230,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="17" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1764,91 +2261,47 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829331A2-8F6C-4EC4-B723-84C59F96FDF0}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:XFD1048576"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{68F8A95A-BB77-4FAE-B840-69C26110AA28}">
-      <formula1>$H$2:$H$5</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68F8A95A-BB77-4FAE-B840-69C26110AA28}">
+          <x14:formula1>
+            <xm:f>TYPES!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1862,71 +2315,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="20" customWidth="1"/>
-    <col min="2" max="4" width="40.85546875" style="20" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="25" style="20" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="20" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="42.42578125" style="15" customWidth="1"/>
+    <col min="2" max="4" width="40.85546875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="25" style="15" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="15" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="42" t="s">
+      <c r="D2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="13" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1941,7 +2394,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C10E56-C51A-4786-825E-CD059CFCA62C}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
@@ -1958,32 +2411,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
@@ -2003,6 +2448,52 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532A997E-8BA5-4F62-858E-EBAD85DF109D}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620E24A2-EABA-41CC-9F0D-AAE22D1E1737}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2024,54 +2515,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2">
         <v>21</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>56.483772999999999</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>-3.1137009999999998</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>157</v>
@@ -2099,7 +2590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2122,154 +2613,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="E7" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>75</v>
+      <c r="G7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2297,574 +2783,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="34">
-        <v>71.257798170000001</v>
-      </c>
-      <c r="D2" s="34">
-        <v>12.857889910000001</v>
-      </c>
-      <c r="E2" s="34">
-        <v>28.588073390000002</v>
-      </c>
-      <c r="F2" s="34">
-        <v>4.686238532</v>
-      </c>
-      <c r="G2" s="35">
-        <v>21.490825690000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="38">
-        <v>71.166972479999998</v>
-      </c>
-      <c r="D3" s="38">
-        <v>15.392110089999999</v>
-      </c>
-      <c r="E3" s="38">
-        <v>13.367889910000001</v>
-      </c>
-      <c r="F3" s="38">
-        <v>6.473394495</v>
-      </c>
-      <c r="G3" s="39">
-        <v>22.334862390000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="34">
-        <v>81.969724769999999</v>
-      </c>
-      <c r="D4" s="34">
-        <v>25.25174312</v>
-      </c>
-      <c r="E4" s="34">
-        <v>25.807339450000001</v>
-      </c>
-      <c r="F4" s="34">
-        <v>5.288990826</v>
-      </c>
-      <c r="G4" s="35">
-        <v>22.637614679999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="38">
-        <v>65.707339450000006</v>
-      </c>
-      <c r="D5" s="38">
-        <v>25.722568809999999</v>
-      </c>
-      <c r="E5" s="38">
-        <v>21.129357800000001</v>
-      </c>
-      <c r="F5" s="38">
-        <v>5.4889908260000002</v>
-      </c>
-      <c r="G5" s="39">
-        <v>25.15045872</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="34">
-        <v>74.703669719999994</v>
-      </c>
-      <c r="D6" s="34">
-        <v>30.143669719999998</v>
-      </c>
-      <c r="E6" s="34">
-        <v>30.366972480000001</v>
-      </c>
-      <c r="F6" s="34">
-        <v>5.923853211</v>
-      </c>
-      <c r="G6" s="35">
-        <v>24.01743119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="38">
-        <v>73.083486239999999</v>
-      </c>
-      <c r="D7" s="38">
-        <v>27.937798170000001</v>
-      </c>
-      <c r="E7" s="38">
-        <v>30</v>
-      </c>
-      <c r="F7" s="38">
-        <v>5.6522935780000001</v>
-      </c>
-      <c r="G7" s="39">
-        <v>25.149541280000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="34">
-        <v>72.968807339999998</v>
-      </c>
-      <c r="D8" s="34">
-        <v>20.827431189999999</v>
-      </c>
-      <c r="E8" s="34">
-        <v>12.22844037</v>
-      </c>
-      <c r="F8" s="34">
-        <v>5.7211009170000002</v>
-      </c>
-      <c r="G8" s="35">
-        <v>23.60642202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="38">
-        <v>76.782568810000001</v>
-      </c>
-      <c r="D9" s="38">
-        <v>14.12577982</v>
-      </c>
-      <c r="E9" s="38">
-        <v>30.302752290000001</v>
-      </c>
-      <c r="F9" s="38">
-        <v>6.2321100920000001</v>
-      </c>
-      <c r="G9" s="39">
-        <v>22.39357798</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="34">
-        <v>71.926605499999994</v>
-      </c>
-      <c r="D10" s="34">
-        <v>18.799449540000001</v>
-      </c>
-      <c r="E10" s="34">
-        <v>31.0293578</v>
-      </c>
-      <c r="F10" s="34">
-        <v>5.1724770639999997</v>
-      </c>
-      <c r="G10" s="35">
-        <v>24.786238529999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="38">
-        <v>68.669724770000002</v>
-      </c>
-      <c r="D11" s="38">
-        <v>30.9287156</v>
-      </c>
-      <c r="E11" s="38">
-        <v>31.1</v>
-      </c>
-      <c r="F11" s="38">
-        <v>5.2853211010000001</v>
-      </c>
-      <c r="G11" s="39">
-        <v>26.860550459999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="34">
-        <v>81.202752290000006</v>
-      </c>
-      <c r="D12" s="34">
-        <v>17.95376147</v>
-      </c>
-      <c r="E12" s="34">
-        <v>26.63853211</v>
-      </c>
-      <c r="F12" s="34">
-        <v>5.2532110090000002</v>
-      </c>
-      <c r="G12" s="35">
-        <v>21.932110089999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="38">
-        <v>70.068807340000006</v>
-      </c>
-      <c r="D13" s="38">
-        <v>19.010183489999999</v>
-      </c>
-      <c r="E13" s="38">
-        <v>31</v>
-      </c>
-      <c r="F13" s="38">
-        <v>5.4633027519999997</v>
-      </c>
-      <c r="G13" s="39">
-        <v>25.90825688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="34">
-        <v>76.370642200000006</v>
-      </c>
-      <c r="D14" s="34">
-        <v>16.138715600000001</v>
-      </c>
-      <c r="E14" s="34">
-        <v>16.18073395</v>
-      </c>
-      <c r="F14" s="34">
-        <v>6.0357798169999999</v>
-      </c>
-      <c r="G14" s="35">
-        <v>19.023853209999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="38">
-        <v>76.220183489999997</v>
-      </c>
-      <c r="D15" s="38">
-        <v>13.73</v>
-      </c>
-      <c r="E15" s="38">
-        <v>25.331192659999999</v>
-      </c>
-      <c r="F15" s="38">
-        <v>5.7688073390000003</v>
-      </c>
-      <c r="G15" s="39">
-        <v>27.56422018</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="34">
-        <v>73.533027520000005</v>
-      </c>
-      <c r="D16" s="34">
-        <v>27.46587156</v>
-      </c>
-      <c r="E16" s="34">
-        <v>31.1</v>
-      </c>
-      <c r="F16" s="34">
-        <v>5.5192660550000001</v>
-      </c>
-      <c r="G16" s="35">
-        <v>27.675229359999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="38">
-        <v>75.496330279999995</v>
-      </c>
-      <c r="D17" s="38">
-        <v>9.9022018349999996</v>
-      </c>
-      <c r="E17" s="38">
-        <v>17.3733945</v>
-      </c>
-      <c r="F17" s="38">
-        <v>5.5954128440000002</v>
-      </c>
-      <c r="G17" s="39">
-        <v>29.033027520000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="34">
-        <v>69.455045870000006</v>
-      </c>
-      <c r="D18" s="34">
-        <v>28.59174312</v>
-      </c>
-      <c r="E18" s="34">
-        <v>30.9</v>
-      </c>
-      <c r="F18" s="34">
-        <v>5.3009174310000002</v>
-      </c>
-      <c r="G18" s="35">
-        <v>20.481651379999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="38">
-        <v>82.181651380000005</v>
-      </c>
-      <c r="D19" s="38">
-        <v>17.993119270000001</v>
-      </c>
-      <c r="E19" s="38">
-        <v>14.49541284</v>
-      </c>
-      <c r="F19" s="38">
-        <v>5.5844036700000004</v>
-      </c>
-      <c r="G19" s="39">
-        <v>29.65321101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="34">
-        <v>60.251376149999999</v>
-      </c>
-      <c r="D20" s="34">
-        <v>12.321376150000001</v>
-      </c>
-      <c r="E20" s="34">
-        <v>16.60917431</v>
-      </c>
-      <c r="F20" s="34">
-        <v>6.3807339450000002</v>
-      </c>
-      <c r="G20" s="35">
-        <v>26.969724769999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="38">
-        <v>73.72752294</v>
-      </c>
-      <c r="D21" s="38">
-        <v>23.482110089999999</v>
-      </c>
-      <c r="E21" s="38">
-        <v>28.159633029999998</v>
-      </c>
-      <c r="F21" s="38">
-        <v>6.1229357799999997</v>
-      </c>
-      <c r="G21" s="39">
-        <v>23.534862390000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="34">
-        <v>72.500917430000001</v>
-      </c>
-      <c r="D22" s="34">
-        <v>11.892752290000001</v>
-      </c>
-      <c r="E22" s="34">
-        <v>29.57706422</v>
-      </c>
-      <c r="F22" s="34">
-        <v>6.1229357799999997</v>
-      </c>
-      <c r="G22" s="35">
-        <v>28.619266060000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="38">
-        <v>68.874311930000005</v>
-      </c>
-      <c r="D23" s="38">
-        <v>21.55614679</v>
-      </c>
-      <c r="E23" s="38">
-        <v>23.639449540000001</v>
-      </c>
-      <c r="F23" s="38">
-        <v>5.4935779819999997</v>
-      </c>
-      <c r="G23" s="39">
-        <v>25.710091739999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A23">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:G1">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Locations on the Y axis and climates (which are described in CLIMATES tab) on the x axis. The actual climate value goes in the matrix cells. See DATA_EXAMPLE tab for more information before completion." sqref="A1" xr:uid="{FC382264-F5BB-4A0A-BB03-320EBF442EFF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Format" prompt="Dates need to be formatted in yyyy-mm-dd format, but the cell type in Excel has to be Text!" sqref="B1" xr:uid="{9F926510-BAE1-4FB0-9AC9-8B05F7299956}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>